<commit_message>
correction mineure (extraction parametre insensible à la casse)
</commit_message>
<xml_diff>
--- a/CV_ref.xlsx
+++ b/CV_ref.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cornet-e\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1E863EA-C362-42DC-A296-5E9AD3005636}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33C24A54-77E9-450F-9A86-3105BC368A10}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="27855" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="66">
   <si>
     <t>Parameter</t>
   </si>
@@ -213,6 +213,12 @@
   </si>
   <si>
     <t>01-07-2025 - 31-07-2025</t>
+  </si>
+  <si>
+    <t>MicroR</t>
+  </si>
+  <si>
+    <t>MacroR</t>
   </si>
 </sst>
 </file>
@@ -575,10 +581,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C119"/>
+  <dimension ref="A1:C121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -877,7 +883,7 @@
         <v>5</v>
       </c>
       <c r="C27">
-        <v>0.3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -888,73 +894,73 @@
         <v>6</v>
       </c>
       <c r="C28">
-        <v>0.3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="B29" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C29">
-        <v>5.03</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="B30" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C30">
-        <v>8.44</v>
+        <v>5.03</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="B31" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C31">
-        <v>1.23</v>
+        <v>8.44</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>14</v>
+        <v>65</v>
       </c>
       <c r="B32" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C32">
-        <v>1.82</v>
+        <v>1.23</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>15</v>
+        <v>65</v>
       </c>
       <c r="B33" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C33">
-        <v>2.83</v>
+        <v>1.82</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>15</v>
+        <v>65</v>
       </c>
       <c r="B34" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C34">
-        <v>1.28</v>
+        <v>1.82</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -962,32 +968,32 @@
         <v>15</v>
       </c>
       <c r="B35" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C35">
-        <v>0.92</v>
+        <v>2.83</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B36" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C36">
-        <v>2.1</v>
+        <v>1.28</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B37" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C37">
-        <v>0.7</v>
+        <v>0.92</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -995,32 +1001,32 @@
         <v>16</v>
       </c>
       <c r="B38" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C38">
-        <v>0.68</v>
+        <v>2.1</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B39" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C39">
-        <v>13.23</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B40" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C40">
-        <v>3.58</v>
+        <v>0.68</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -1028,32 +1034,32 @@
         <v>17</v>
       </c>
       <c r="B41" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C41">
-        <v>3.09</v>
+        <v>13.23</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B42" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C42">
-        <v>5.72</v>
+        <v>3.58</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B43" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C43">
-        <v>1.58</v>
+        <v>3.09</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -1061,32 +1067,32 @@
         <v>18</v>
       </c>
       <c r="B44" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C44">
-        <v>0.72</v>
+        <v>5.72</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B45" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C45">
-        <v>1.27</v>
+        <v>1.58</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B46" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C46">
-        <v>0.92</v>
+        <v>0.72</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -1094,32 +1100,32 @@
         <v>19</v>
       </c>
       <c r="B47" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C47">
-        <v>0.44</v>
+        <v>1.27</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B48" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C48">
-        <v>3.07</v>
+        <v>0.92</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B49" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C49">
-        <v>1.94</v>
+        <v>0.44</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -1127,32 +1133,32 @@
         <v>20</v>
       </c>
       <c r="B50" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C50">
-        <v>1.6</v>
+        <v>3.07</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B51" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C51">
-        <v>2.8</v>
+        <v>1.94</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B52" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C52">
-        <v>1.86</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -1160,32 +1166,32 @@
         <v>21</v>
       </c>
       <c r="B53" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C53">
-        <v>1.56</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B54" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C54">
-        <v>6.51</v>
+        <v>1.86</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B55" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C55">
-        <v>3.08</v>
+        <v>1.56</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -1193,32 +1199,32 @@
         <v>22</v>
       </c>
       <c r="B56" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C56">
-        <v>1.75</v>
+        <v>6.51</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B57" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C57">
-        <v>6.56</v>
+        <v>3.08</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B58" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C58">
-        <v>3.4</v>
+        <v>1.75</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -1226,32 +1232,32 @@
         <v>23</v>
       </c>
       <c r="B59" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C59">
-        <v>1.84</v>
+        <v>6.56</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B60" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C60">
-        <v>1.52</v>
+        <v>3.4</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B61" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C61">
-        <v>0.67</v>
+        <v>1.84</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -1259,32 +1265,32 @@
         <v>24</v>
       </c>
       <c r="B62" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C62">
-        <v>0.57999999999999996</v>
+        <v>1.52</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B63" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C63">
-        <v>1.9</v>
+        <v>0.67</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B64" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C64">
-        <v>1.33</v>
+        <v>0.57999999999999996</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -1292,32 +1298,32 @@
         <v>25</v>
       </c>
       <c r="B65" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C65">
-        <v>1.1299999999999999</v>
+        <v>1.9</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B66" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C66">
-        <v>1.38</v>
+        <v>1.33</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B67" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C67">
-        <v>0.85</v>
+        <v>1.1299999999999999</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -1325,32 +1331,32 @@
         <v>26</v>
       </c>
       <c r="B68" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C68">
-        <v>1.1200000000000001</v>
+        <v>1.38</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B69" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C69">
-        <v>3.87</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B70" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C70">
-        <v>2.62</v>
+        <v>1.1200000000000001</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
@@ -1358,32 +1364,32 @@
         <v>27</v>
       </c>
       <c r="B71" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C71">
-        <v>4.51</v>
+        <v>3.87</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B72" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C72">
-        <v>3.55</v>
+        <v>2.62</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B73" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C73">
-        <v>2.58</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
@@ -1391,32 +1397,32 @@
         <v>28</v>
       </c>
       <c r="B74" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C74">
-        <v>4.42</v>
+        <v>3.55</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B75" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C75">
-        <v>1.83</v>
+        <v>2.58</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B76" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C76">
-        <v>1.41</v>
+        <v>4.42</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
@@ -1424,32 +1430,32 @@
         <v>29</v>
       </c>
       <c r="B77" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C77">
-        <v>1</v>
+        <v>1.83</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B78" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C78">
-        <v>1.54</v>
+        <v>1.41</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B79" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C79">
-        <v>1.1000000000000001</v>
+        <v>1</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
@@ -1457,32 +1463,32 @@
         <v>30</v>
       </c>
       <c r="B80" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C80">
-        <v>0.85</v>
+        <v>1.54</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B81" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C81">
-        <v>4.53</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B82" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C82">
-        <v>2.04</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
@@ -1490,32 +1496,32 @@
         <v>31</v>
       </c>
       <c r="B83" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C83">
-        <v>1.65</v>
+        <v>4.53</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B84" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C84">
-        <v>4.34</v>
+        <v>2.04</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B85" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C85">
-        <v>1.82</v>
+        <v>1.65</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
@@ -1523,32 +1529,32 @@
         <v>32</v>
       </c>
       <c r="B86" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C86">
-        <v>1.66</v>
+        <v>4.34</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B87" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C87">
-        <v>1.85</v>
+        <v>1.82</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B88" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C88">
-        <v>1.77</v>
+        <v>1.66</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
@@ -1556,32 +1562,32 @@
         <v>33</v>
       </c>
       <c r="B89" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C89">
-        <v>1.59</v>
+        <v>1.85</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B90" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C90">
-        <v>1.88</v>
+        <v>1.77</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B91" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C91">
-        <v>1.27</v>
+        <v>1.59</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
@@ -1589,32 +1595,32 @@
         <v>34</v>
       </c>
       <c r="B92" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C92">
-        <v>1.54</v>
+        <v>1.88</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B93" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C93">
-        <v>0.18</v>
+        <v>1.27</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B94" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C94">
-        <v>0.13</v>
+        <v>1.54</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
@@ -1622,32 +1628,32 @@
         <v>35</v>
       </c>
       <c r="B95" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C95">
-        <v>0.09</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B96" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C96">
-        <v>1.58</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B97" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C97">
-        <v>1.29</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
@@ -1655,32 +1661,32 @@
         <v>36</v>
       </c>
       <c r="B98" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C98">
-        <v>1.6</v>
+        <v>1.58</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B99" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C99">
-        <v>2.5099999999999998</v>
+        <v>1.29</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B100" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C100">
-        <v>2.11</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
@@ -1688,32 +1694,32 @@
         <v>37</v>
       </c>
       <c r="B101" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C101">
-        <v>2.12</v>
+        <v>2.5099999999999998</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B102" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C102">
-        <v>2.23</v>
+        <v>2.11</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B103" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C103">
-        <v>1.55</v>
+        <v>2.12</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
@@ -1721,32 +1727,32 @@
         <v>38</v>
       </c>
       <c r="B104" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C104">
-        <v>2.13</v>
+        <v>2.23</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B105" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C105">
-        <v>2.56</v>
+        <v>1.55</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B106" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C106">
-        <v>1.88</v>
+        <v>2.13</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
@@ -1754,32 +1760,32 @@
         <v>39</v>
       </c>
       <c r="B107" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C107">
-        <v>1.75</v>
+        <v>2.56</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B108" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C108">
-        <v>2.42</v>
+        <v>1.88</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B109" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C109">
-        <v>1.86</v>
+        <v>1.75</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
@@ -1787,32 +1793,32 @@
         <v>40</v>
       </c>
       <c r="B110" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C110">
-        <v>1.62</v>
+        <v>2.42</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B111" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C111">
-        <v>0.18</v>
+        <v>1.86</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B112" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C112">
-        <v>0.13</v>
+        <v>1.62</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
@@ -1820,32 +1826,32 @@
         <v>41</v>
       </c>
       <c r="B113" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C113">
-        <v>0.09</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B114" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C114">
-        <v>1.58</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B115" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C115">
-        <v>1.29</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
@@ -1853,32 +1859,32 @@
         <v>42</v>
       </c>
       <c r="B116" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C116">
-        <v>1.6</v>
+        <v>1.58</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B117" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C117">
-        <v>0.48</v>
+        <v>1.29</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B118" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C118">
-        <v>0.23</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
@@ -1886,9 +1892,31 @@
         <v>43</v>
       </c>
       <c r="B119" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C119">
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>43</v>
+      </c>
+      <c r="B120" t="s">
+        <v>5</v>
+      </c>
+      <c r="C120">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>43</v>
+      </c>
+      <c r="B121" t="s">
+        <v>6</v>
+      </c>
+      <c r="C121">
         <v>0.22</v>
       </c>
     </row>

</xml_diff>